<commit_message>
Slightly changed a header
moved t into header in both demand and storage page
</commit_message>
<xml_diff>
--- a/Spine_Projects/Maersk_Example/Input/Maersk_Example_Dana.xlsx
+++ b/Spine_Projects/Maersk_Example/Input/Maersk_Example_Dana.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/dahe23af_student_cbs_dk/Documents/Dokumente/GitHub/Nord_H2ub/Spine_Projects/Maersk_Example/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{CCFD4AEF-1C80-4751-9EC4-653C8BA7E1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3A7ABA5-4CF2-476B-843B-F26346619160}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{CCFD4AEF-1C80-4751-9EC4-653C8BA7E1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{264E148D-9C2B-42C4-872E-7EADC0C8D6AC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="8" xr2:uid="{51DBCAFA-CEB1-4B3C-966C-9DE7E0983FEC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="7" xr2:uid="{51DBCAFA-CEB1-4B3C-966C-9DE7E0983FEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="2" r:id="rId1"/>
@@ -2136,7 +2136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23586A81-B41F-419A-9CC9-DCB1E38C3013}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -2153,6 +2153,9 @@
       <c r="B1" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="J1" s="2" t="s">
         <v>73</v>
       </c>
@@ -2180,9 +2183,6 @@
       </c>
       <c r="B3">
         <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
       </c>
       <c r="J3" t="s">
         <v>98</v>
@@ -2279,7 +2279,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4937129D-37FF-4EB7-B39E-7B40CC16C5CB}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2288,6 +2290,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>74</v>
       </c>
@@ -2296,9 +2301,6 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>28</v>
-      </c>
       <c r="B2" t="s">
         <v>97</v>
       </c>
@@ -2545,6 +2547,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="edf6ee90-b14e-4711-bf2d-b1beadcb41f5">
@@ -2553,15 +2564,6 @@
     <TaxCatchAll xmlns="588af687-a5f4-46dc-9eef-8f2d5661ca5c" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2584,6 +2586,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076CFCCE-199C-443B-B7C0-D7012460C8B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A615901B-11F2-4C79-A718-E36071167164}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2592,12 +2602,4 @@
     <ds:schemaRef ds:uri="588af687-a5f4-46dc-9eef-8f2d5661ca5c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076CFCCE-199C-443B-B7C0-D7012460C8B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add further model components
</commit_message>
<xml_diff>
--- a/Spine_Projects/Maersk_Example/Input/Maersk_Example_Dana.xlsx
+++ b/Spine_Projects/Maersk_Example/Input/Maersk_Example_Dana.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Maersk_Example\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD697765-651D-4519-A427-18F04C89FF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E8A0AF-D557-4C80-8CEF-D4558A793250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="7" xr2:uid="{51DBCAFA-CEB1-4B3C-966C-9DE7E0983FEC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="7" xr2:uid="{51DBCAFA-CEB1-4B3C-966C-9DE7E0983FEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="101">
   <si>
     <t>Object_Class_Name</t>
   </si>
@@ -344,6 +344,12 @@
   </si>
   <si>
     <t>demand</t>
+  </si>
+  <si>
+    <t>unit_availibility_factor</t>
+  </si>
+  <si>
+    <t>tax_out_unit_flow</t>
   </si>
 </sst>
 </file>
@@ -707,7 +713,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E06231-8D06-41D8-8548-8EF76320D96E}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2119,10 +2127,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23586A81-B41F-419A-9CC9-DCB1E38C3013}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2134,23 +2142,35 @@
     <col min="11" max="11" width="16.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2160,8 +2180,14 @@
       <c r="C3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -2171,8 +2197,14 @@
       <c r="C4">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -2182,8 +2214,14 @@
       <c r="C5">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>0.2</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -2193,8 +2231,14 @@
       <c r="C6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>0.8</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -2204,8 +2248,14 @@
       <c r="C7">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <v>0.3</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2214,6 +2264,12 @@
       </c>
       <c r="C8">
         <v>50</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleted Demand for Hydrogen
Both Excel and Data Store are updated
</commit_message>
<xml_diff>
--- a/Spine_Projects/Maersk_Example/Input/Maersk_Example_Dana.xlsx
+++ b/Spine_Projects/Maersk_Example/Input/Maersk_Example_Dana.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/dahe23af_student_cbs_dk/Documents/Dokumente/GitHub/Nord_H2ub/Spine_Projects/Maersk_Example/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{345F95B6-B533-4C72-9D60-70BBA323E5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B957F285-E746-4D59-9E8F-F80D6EFBDC1E}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{345F95B6-B533-4C72-9D60-70BBA323E5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C4212AC-DA4D-4DEF-A09F-188D32FF8A69}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{51DBCAFA-CEB1-4B3C-966C-9DE7E0983FEC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{51DBCAFA-CEB1-4B3C-966C-9DE7E0983FEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="2" r:id="rId1"/>
@@ -716,9 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E06231-8D06-41D8-8548-8EF76320D96E}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -798,9 +796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0FFD16-F425-46EA-BE6D-7390D00C1F7D}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -881,9 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECF8EFB-268E-462A-9798-31D873EE5EEE}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1204,9 +1198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A799C4-DA9C-4714-A630-723B6360198C}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1435,9 +1427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608168D5-0738-458F-A88D-26E31671DE43}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1514,9 +1504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8198CF-B8BA-4E3C-BDFC-CD95322E57D9}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1714,9 +1702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7C13A2-FD8E-478F-BA61-51475C93DC7E}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1875,9 +1861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1643F6E4-3605-4383-8FB3-5670E91EAFE9}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2036,9 +2020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBA0A5B-E4FE-413F-8B3A-7F0B2236AD9D}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2158,14 +2140,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23586A81-B41F-419A-9CC9-DCB1E38C3013}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.36328125" bestFit="1" customWidth="1"/>
@@ -2174,6 +2155,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>73</v>
       </c>
@@ -2202,9 +2186,6 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
       <c r="B3" t="s">
         <v>97</v>
       </c>
@@ -2223,10 +2204,10 @@
         <v>29</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>20</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -2240,10 +2221,10 @@
         <v>30</v>
       </c>
       <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>20</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
       </c>
       <c r="D5">
         <v>0.2</v>
@@ -2257,10 +2238,10 @@
         <v>31</v>
       </c>
       <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>30</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
       </c>
       <c r="D6">
         <v>0.8</v>
@@ -2274,10 +2255,10 @@
         <v>32</v>
       </c>
       <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>20</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
       </c>
       <c r="D7">
         <v>0.3</v>
@@ -2291,10 +2272,10 @@
         <v>33</v>
       </c>
       <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
         <v>25</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -2312,9 +2293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4937129D-37FF-4EB7-B39E-7B40CC16C5CB}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2378,6 +2357,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="edf6ee90-b14e-4711-bf2d-b1beadcb41f5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="588af687-a5f4-46dc-9eef-8f2d5661ca5c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B227512146E4794EA3DFC577899B9574" ma:contentTypeVersion="11" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="102f62f00864d00911f0d8ac363b6ca3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="edf6ee90-b14e-4711-bf2d-b1beadcb41f5" xmlns:ns3="588af687-a5f4-46dc-9eef-8f2d5661ca5c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3a87685c95b9a647e91677dfbca7cf1" ns2:_="" ns3:_="">
     <xsd:import namespace="edf6ee90-b14e-4711-bf2d-b1beadcb41f5"/>
@@ -2588,17 +2578,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="edf6ee90-b14e-4711-bf2d-b1beadcb41f5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="588af687-a5f4-46dc-9eef-8f2d5661ca5c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{076CFCCE-199C-443B-B7C0-D7012460C8B3}">
   <ds:schemaRefs>
@@ -2608,6 +2587,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A615901B-11F2-4C79-A718-E36071167164}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="edf6ee90-b14e-4711-bf2d-b1beadcb41f5"/>
+    <ds:schemaRef ds:uri="588af687-a5f4-46dc-9eef-8f2d5661ca5c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A8D886F-66F0-418B-866D-5835753D7F21}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2624,15 +2614,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A615901B-11F2-4C79-A718-E36071167164}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="edf6ee90-b14e-4711-bf2d-b1beadcb41f5"/>
-    <ds:schemaRef ds:uri="588af687-a5f4-46dc-9eef-8f2d5661ca5c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>